<commit_message>
now max length of author and song name computed dinamically depending on the opened folder
</commit_message>
<xml_diff>
--- a/Blopnote/blopnote bugs.xlsx
+++ b/Blopnote/blopnote bugs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azgel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azgel\source\repos\Blopnote\Blopnote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF350DE-DB4A-42D2-9892-9AFECC121B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5D8F3E-BB2A-461C-9669-533DF7B50795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D1902E2-70B7-47CB-86DF-C5450FDE41FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -156,12 +156,6 @@
     <t>I changed my mind</t>
   </si>
   <si>
-    <t>I don't understand how to invoke it. it invokes only for rare files.</t>
-  </si>
-  <si>
-    <t>i just changed the both maxlengths to 100 but lyrics still yield returns and ohh, i just remembered it</t>
-  </si>
-  <si>
     <t>lyrics</t>
   </si>
   <si>
@@ -193,6 +187,33 @@
   </si>
   <si>
     <t>info specified but messagebox looks awkward. I'd better highlight empty fields after click on OK</t>
+  </si>
+  <si>
+    <t>no setting for auto-save interval</t>
+  </si>
+  <si>
+    <t>I don't understand how to invoke it. it invokes rarely</t>
+  </si>
+  <si>
+    <t>too long loading</t>
+  </si>
+  <si>
+    <t>bottom half/part of lyrics could disappear</t>
+  </si>
+  <si>
+    <t>when open/close many files than lyrics displayed incorrect and when you scroll scrollbar lyrics appears at mid of app but must at the bottom of app</t>
+  </si>
+  <si>
+    <t>i just changed the both maxlengths to 100 but lyrics still yield error. ohh, i've understood. the max length of FILE_PATH in windows 10 is 255 characters. so the max length of file has to depend on the current directory path length so max length of textboxes in create form must be dynamically changable.So i implemented dinamically changing in 30 mins</t>
+  </si>
+  <si>
+    <t>what folder is opened now?</t>
+  </si>
+  <si>
+    <t>it's hard to understand to user what folder is opened in app right now. To do it he can click the  "Open" button and current folder will be opend but it's so hard for newbie</t>
+  </si>
+  <si>
+    <t>I could add to programstatus bottom bar information about it</t>
   </si>
 </sst>
 </file>
@@ -602,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5A6968-05AB-409C-B696-8DB44652D9F9}">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,10 +660,10 @@
         <v>37</v>
       </c>
       <c r="N1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -663,13 +684,13 @@
       </c>
       <c r="F2" s="6"/>
       <c r="N2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -690,13 +711,13 @@
       </c>
       <c r="F3" s="6"/>
       <c r="N3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -718,13 +739,13 @@
         <v>38</v>
       </c>
       <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" t="s">
         <v>47</v>
-      </c>
-      <c r="O4" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -745,16 +766,16 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="4" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="N5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -771,7 +792,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F6" s="6"/>
     </row>
@@ -787,7 +808,7 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="4" t="s">
@@ -802,7 +823,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>19</v>
@@ -812,10 +833,10 @@
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -848,7 +869,7 @@
         <v>21</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -870,7 +891,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="210" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -888,7 +909,7 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="4" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -923,7 +944,7 @@
         <v>31</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -939,7 +960,7 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -990,7 +1011,9 @@
       <c r="D18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="4" t="s">
         <v>41</v>
@@ -1001,56 +1024,89 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F23" s="1"/>
+      <c r="G23" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5">

</xml_diff>